<commit_message>
2nd checkin to test git tracking
</commit_message>
<xml_diff>
--- a/Rakesh_SNOW.xlsx
+++ b/Rakesh_SNOW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rakesh\Downloads\Tech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288828DD-673B-4BEF-99D8-7A7A627D20B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8467FDEA-E4C3-42CE-A41C-7E93701CDF3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3656" uniqueCount="809">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3657" uniqueCount="810">
   <si>
     <t>Opened</t>
   </si>
@@ -3124,6 +3124,9 @@
   </si>
   <si>
     <t>testing git</t>
+  </si>
+  <si>
+    <t>testing git 2</t>
   </si>
 </sst>
 </file>
@@ -17088,17 +17091,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5552C989-3B06-4CC5-BC8F-50E76992BBFA}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.69921875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>808</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>809</v>
       </c>
     </row>
   </sheetData>
@@ -17113,6 +17124,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006C64CDFB56E89048996B9D42780A3BDE" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a27aa52844f394a89ad83f72ada0fb09">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="35360bb6-9540-4669-93c9-f83b5cf64b17" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1e626a048a0a6ca75be6698de65087d6" ns3:_="">
     <xsd:import namespace="35360bb6-9540-4669-93c9-f83b5cf64b17"/>
@@ -17290,15 +17310,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F26F6FFB-9E3D-4A05-9B7E-891284A30079}">
   <ds:schemaRefs>
@@ -17316,6 +17327,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{990F9785-C3BE-4B58-A8AA-A0B0C15AA7D7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD4A6D94-67A3-4F45-AB1D-0614C945EA52}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17331,12 +17350,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{990F9785-C3BE-4B58-A8AA-A0B0C15AA7D7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>